<commit_message>
fixed front end with validation
</commit_message>
<xml_diff>
--- a/pythonCW/test.xlsx
+++ b/pythonCW/test.xlsx
@@ -26392,13 +26392,21 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I102"/>
+  <dimension ref="A1:F102"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="9.6" customWidth="1" min="1" max="1"/>
+    <col width="14.4" customWidth="1" min="2" max="2"/>
+    <col width="10.8" customWidth="1" min="3" max="3"/>
+    <col width="16.8" customWidth="1" min="4" max="4"/>
+    <col width="4.8" customWidth="1" min="5" max="5"/>
+    <col width="4.8" customWidth="1" min="6" max="6"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="2" t="inlineStr">
@@ -26423,2928 +26431,2013 @@
       </c>
       <c r="E1" s="2" t="inlineStr">
         <is>
-          <t>USA_w</t>
+          <t>w1</t>
         </is>
       </c>
       <c r="F1" s="2" t="inlineStr">
         <is>
-          <t>UK_w</t>
-        </is>
-      </c>
-      <c r="G1" s="2" t="inlineStr">
-        <is>
-          <t>SWITZERLAND_w</t>
-        </is>
-      </c>
-      <c r="H1" s="2" t="inlineStr">
-        <is>
-          <t>JAPAN_w</t>
-        </is>
-      </c>
-      <c r="I1" s="2" t="inlineStr">
-        <is>
-          <t>CANADA_w</t>
+          <t>w2</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>0.0994</v>
+        <v>0.1601</v>
       </c>
       <c r="B2" t="n">
-        <v>0.1428</v>
+        <v>0.2118</v>
       </c>
       <c r="C2" t="n">
-        <v>0.0688</v>
+        <v>0.09279999999999999</v>
       </c>
       <c r="D2" t="n">
-        <v>0.5558</v>
+        <v>0.5433</v>
       </c>
       <c r="E2" t="n">
-        <v>0.6591</v>
+        <v>0.0721</v>
       </c>
       <c r="F2" t="n">
-        <v>-0.253</v>
-      </c>
-      <c r="G2" t="n">
-        <v>0.5077</v>
-      </c>
-      <c r="H2" t="n">
-        <v>0.2533</v>
-      </c>
-      <c r="I2" t="n">
-        <v>-0.1671</v>
+        <v>0.9278999999999999</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>0.09950000000000001</v>
+        <v>0.1601</v>
       </c>
       <c r="B3" t="n">
-        <v>0.1428</v>
+        <v>0.2118</v>
       </c>
       <c r="C3" t="n">
-        <v>0.0689</v>
+        <v>0.0929</v>
       </c>
       <c r="D3" t="n">
-        <v>0.5564</v>
+        <v>0.5436</v>
       </c>
       <c r="E3" t="n">
-        <v>0.6604</v>
+        <v>0.073</v>
       </c>
       <c r="F3" t="n">
-        <v>-0.2541</v>
-      </c>
-      <c r="G3" t="n">
-        <v>0.5081</v>
-      </c>
-      <c r="H3" t="n">
-        <v>0.2527</v>
-      </c>
-      <c r="I3" t="n">
-        <v>-0.167</v>
+        <v>0.927</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>0.09950000000000001</v>
+        <v>0.1603</v>
       </c>
       <c r="B4" t="n">
-        <v>0.1428</v>
+        <v>0.2114</v>
       </c>
       <c r="C4" t="n">
-        <v>0.0689</v>
+        <v>0.09320000000000001</v>
       </c>
       <c r="D4" t="n">
-        <v>0.5567</v>
+        <v>0.5451</v>
       </c>
       <c r="E4" t="n">
-        <v>0.661</v>
+        <v>0.0769</v>
       </c>
       <c r="F4" t="n">
-        <v>-0.2547</v>
-      </c>
-      <c r="G4" t="n">
-        <v>0.5083</v>
-      </c>
-      <c r="H4" t="n">
-        <v>0.2524</v>
-      </c>
-      <c r="I4" t="n">
-        <v>-0.1669</v>
+        <v>0.9231</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>0.0997</v>
+        <v>0.1603</v>
       </c>
       <c r="B5" t="n">
-        <v>0.1428</v>
+        <v>0.2112</v>
       </c>
       <c r="C5" t="n">
-        <v>0.0692</v>
+        <v>0.0934</v>
       </c>
       <c r="D5" t="n">
-        <v>0.5584</v>
+        <v>0.5461</v>
       </c>
       <c r="E5" t="n">
-        <v>0.6647</v>
+        <v>0.0793</v>
       </c>
       <c r="F5" t="n">
-        <v>-0.2582</v>
-      </c>
-      <c r="G5" t="n">
-        <v>0.5094</v>
-      </c>
-      <c r="H5" t="n">
-        <v>0.2505</v>
-      </c>
-      <c r="I5" t="n">
-        <v>-0.1665</v>
+        <v>0.9207</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>0.0998</v>
+        <v>0.1606</v>
       </c>
       <c r="B6" t="n">
-        <v>0.1428</v>
+        <v>0.2106</v>
       </c>
       <c r="C6" t="n">
-        <v>0.0692</v>
+        <v>0.0941</v>
       </c>
       <c r="D6" t="n">
-        <v>0.5590000000000001</v>
+        <v>0.5491</v>
       </c>
       <c r="E6" t="n">
-        <v>0.666</v>
+        <v>0.0872</v>
       </c>
       <c r="F6" t="n">
-        <v>-0.2594</v>
-      </c>
-      <c r="G6" t="n">
-        <v>0.5098</v>
-      </c>
-      <c r="H6" t="n">
-        <v>0.2499</v>
-      </c>
-      <c r="I6" t="n">
-        <v>-0.1663</v>
+        <v>0.9127999999999999</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>0.1002</v>
+        <v>0.1608</v>
       </c>
       <c r="B7" t="n">
-        <v>0.1428</v>
+        <v>0.2103</v>
       </c>
       <c r="C7" t="n">
-        <v>0.0696</v>
+        <v>0.0945</v>
       </c>
       <c r="D7" t="n">
-        <v>0.5619</v>
+        <v>0.5506</v>
       </c>
       <c r="E7" t="n">
-        <v>0.6722</v>
+        <v>0.09130000000000001</v>
       </c>
       <c r="F7" t="n">
-        <v>-0.2652</v>
-      </c>
-      <c r="G7" t="n">
-        <v>0.5118</v>
-      </c>
-      <c r="H7" t="n">
-        <v>0.2468</v>
-      </c>
-      <c r="I7" t="n">
-        <v>-0.1656</v>
+        <v>0.9087</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>0.1003</v>
+        <v>0.1612</v>
       </c>
       <c r="B8" t="n">
-        <v>0.1428</v>
+        <v>0.2094</v>
       </c>
       <c r="C8" t="n">
-        <v>0.0698</v>
+        <v>0.0954</v>
       </c>
       <c r="D8" t="n">
-        <v>0.5627</v>
+        <v>0.555</v>
       </c>
       <c r="E8" t="n">
-        <v>0.6741</v>
+        <v>0.1031</v>
       </c>
       <c r="F8" t="n">
-        <v>-0.2669</v>
-      </c>
-      <c r="G8" t="n">
-        <v>0.5124</v>
-      </c>
-      <c r="H8" t="n">
-        <v>0.2459</v>
-      </c>
-      <c r="I8" t="n">
-        <v>-0.1654</v>
+        <v>0.8969</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>0.1009</v>
+        <v>0.1614</v>
       </c>
       <c r="B9" t="n">
-        <v>0.1428</v>
+        <v>0.209</v>
       </c>
       <c r="C9" t="n">
-        <v>0.0703</v>
+        <v>0.0959</v>
       </c>
       <c r="D9" t="n">
-        <v>0.5667</v>
+        <v>0.5570000000000001</v>
       </c>
       <c r="E9" t="n">
-        <v>0.6828</v>
+        <v>0.1088</v>
       </c>
       <c r="F9" t="n">
-        <v>-0.2751</v>
-      </c>
-      <c r="G9" t="n">
-        <v>0.5151</v>
-      </c>
-      <c r="H9" t="n">
-        <v>0.2416</v>
-      </c>
-      <c r="I9" t="n">
-        <v>-0.1644</v>
+        <v>0.8912</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>0.1011</v>
+        <v>0.162</v>
       </c>
       <c r="B10" t="n">
-        <v>0.1428</v>
+        <v>0.2079</v>
       </c>
       <c r="C10" t="n">
-        <v>0.07049999999999999</v>
+        <v>0.09710000000000001</v>
       </c>
       <c r="D10" t="n">
-        <v>0.5678</v>
+        <v>0.5626</v>
       </c>
       <c r="E10" t="n">
-        <v>0.6853</v>
+        <v>0.1246</v>
       </c>
       <c r="F10" t="n">
-        <v>-0.2774</v>
-      </c>
-      <c r="G10" t="n">
-        <v>0.5159</v>
-      </c>
-      <c r="H10" t="n">
-        <v>0.2403</v>
-      </c>
-      <c r="I10" t="n">
-        <v>-0.1641</v>
+        <v>0.8754</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>0.1018</v>
+        <v>0.1622</v>
       </c>
       <c r="B11" t="n">
-        <v>0.1428</v>
+        <v>0.2075</v>
       </c>
       <c r="C11" t="n">
-        <v>0.0712</v>
+        <v>0.0977</v>
       </c>
       <c r="D11" t="n">
-        <v>0.5729</v>
+        <v>0.5651</v>
       </c>
       <c r="E11" t="n">
-        <v>0.6965</v>
+        <v>0.1319</v>
       </c>
       <c r="F11" t="n">
-        <v>-0.2878</v>
-      </c>
-      <c r="G11" t="n">
-        <v>0.5194</v>
-      </c>
-      <c r="H11" t="n">
-        <v>0.2348</v>
-      </c>
-      <c r="I11" t="n">
-        <v>-0.1628</v>
+        <v>0.8681</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>0.102</v>
+        <v>0.1629</v>
       </c>
       <c r="B12" t="n">
-        <v>0.1428</v>
+        <v>0.2064</v>
       </c>
       <c r="C12" t="n">
-        <v>0.07140000000000001</v>
+        <v>0.09909999999999999</v>
       </c>
       <c r="D12" t="n">
-        <v>0.5743</v>
+        <v>0.5715</v>
       </c>
       <c r="E12" t="n">
-        <v>0.6996</v>
+        <v>0.1516</v>
       </c>
       <c r="F12" t="n">
-        <v>-0.2907</v>
-      </c>
-      <c r="G12" t="n">
-        <v>0.5204</v>
-      </c>
-      <c r="H12" t="n">
-        <v>0.2332</v>
-      </c>
-      <c r="I12" t="n">
-        <v>-0.1625</v>
+        <v>0.8484</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>0.1029</v>
+        <v>0.1633</v>
       </c>
       <c r="B13" t="n">
-        <v>0.1428</v>
+        <v>0.2059</v>
       </c>
       <c r="C13" t="n">
-        <v>0.0723</v>
+        <v>0.0997</v>
       </c>
       <c r="D13" t="n">
-        <v>0.5805</v>
+        <v>0.5743</v>
       </c>
       <c r="E13" t="n">
-        <v>0.7134</v>
+        <v>0.1606</v>
       </c>
       <c r="F13" t="n">
-        <v>-0.3035</v>
-      </c>
-      <c r="G13" t="n">
-        <v>0.5247000000000001</v>
-      </c>
-      <c r="H13" t="n">
-        <v>0.2264</v>
-      </c>
-      <c r="I13" t="n">
-        <v>-0.1609</v>
+        <v>0.8394</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>0.1041</v>
+        <v>0.1641</v>
       </c>
       <c r="B14" t="n">
-        <v>0.1428</v>
+        <v>0.2049</v>
       </c>
       <c r="C14" t="n">
-        <v>0.0736</v>
+        <v>0.1011</v>
       </c>
       <c r="D14" t="n">
-        <v>0.5893</v>
+        <v>0.5813</v>
       </c>
       <c r="E14" t="n">
-        <v>0.7333</v>
+        <v>0.1842</v>
       </c>
       <c r="F14" t="n">
-        <v>-0.3221</v>
-      </c>
-      <c r="G14" t="n">
-        <v>0.5309</v>
-      </c>
-      <c r="H14" t="n">
-        <v>0.2165</v>
-      </c>
-      <c r="I14" t="n">
-        <v>-0.1586</v>
+        <v>0.8158</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>0.1056</v>
+        <v>0.1645</v>
       </c>
       <c r="B15" t="n">
-        <v>0.1429</v>
+        <v>0.2045</v>
       </c>
       <c r="C15" t="n">
-        <v>0.075</v>
+        <v>0.1017</v>
       </c>
       <c r="D15" t="n">
-        <v>0.5993000000000001</v>
+        <v>0.5842000000000001</v>
       </c>
       <c r="E15" t="n">
-        <v>0.7564</v>
+        <v>0.1949</v>
       </c>
       <c r="F15" t="n">
-        <v>-0.3436</v>
-      </c>
-      <c r="G15" t="n">
-        <v>0.5382</v>
-      </c>
-      <c r="H15" t="n">
-        <v>0.2051</v>
-      </c>
-      <c r="I15" t="n">
-        <v>-0.156</v>
+        <v>0.8051</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>0.1073</v>
+        <v>0.1655</v>
       </c>
       <c r="B16" t="n">
-        <v>0.143</v>
+        <v>0.2038</v>
       </c>
       <c r="C16" t="n">
-        <v>0.0766</v>
+        <v>0.1032</v>
       </c>
       <c r="D16" t="n">
-        <v>0.6104000000000001</v>
+        <v>0.5911</v>
       </c>
       <c r="E16" t="n">
-        <v>0.7826</v>
+        <v>0.2224</v>
       </c>
       <c r="F16" t="n">
-        <v>-0.368</v>
-      </c>
-      <c r="G16" t="n">
-        <v>0.5464</v>
-      </c>
-      <c r="H16" t="n">
-        <v>0.1921</v>
-      </c>
-      <c r="I16" t="n">
-        <v>-0.153</v>
+        <v>0.7776</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>0.1092</v>
+        <v>0.1659</v>
       </c>
       <c r="B17" t="n">
-        <v>0.1432</v>
+        <v>0.2036</v>
       </c>
       <c r="C17" t="n">
-        <v>0.0784</v>
+        <v>0.1037</v>
       </c>
       <c r="D17" t="n">
-        <v>0.6226</v>
+        <v>0.5939</v>
       </c>
       <c r="E17" t="n">
-        <v>0.8119</v>
+        <v>0.2347</v>
       </c>
       <c r="F17" t="n">
-        <v>-0.3953</v>
-      </c>
-      <c r="G17" t="n">
-        <v>0.5555</v>
-      </c>
-      <c r="H17" t="n">
-        <v>0.1776</v>
-      </c>
-      <c r="I17" t="n">
-        <v>-0.1497</v>
+        <v>0.7653</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>0.1113</v>
+        <v>0.1671</v>
       </c>
       <c r="B18" t="n">
-        <v>0.1436</v>
+        <v>0.2034</v>
       </c>
       <c r="C18" t="n">
-        <v>0.0803</v>
+        <v>0.105</v>
       </c>
       <c r="D18" t="n">
-        <v>0.6357</v>
+        <v>0.6001</v>
       </c>
       <c r="E18" t="n">
-        <v>0.8443000000000001</v>
+        <v>0.2661</v>
       </c>
       <c r="F18" t="n">
-        <v>-0.4256</v>
-      </c>
-      <c r="G18" t="n">
-        <v>0.5657</v>
-      </c>
-      <c r="H18" t="n">
-        <v>0.1615</v>
-      </c>
-      <c r="I18" t="n">
-        <v>-0.146</v>
+        <v>0.7339</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>0.1135</v>
+        <v>0.1676</v>
       </c>
       <c r="B19" t="n">
-        <v>0.144</v>
+        <v>0.2034</v>
       </c>
       <c r="C19" t="n">
-        <v>0.0824</v>
+        <v>0.1055</v>
       </c>
       <c r="D19" t="n">
-        <v>0.6495</v>
+        <v>0.6024</v>
       </c>
       <c r="E19" t="n">
-        <v>0.8798</v>
+        <v>0.2801</v>
       </c>
       <c r="F19" t="n">
-        <v>-0.4587</v>
-      </c>
-      <c r="G19" t="n">
-        <v>0.5768</v>
-      </c>
-      <c r="H19" t="n">
-        <v>0.1439</v>
-      </c>
-      <c r="I19" t="n">
-        <v>-0.1419</v>
+        <v>0.7199</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>0.116</v>
+        <v>0.1694</v>
       </c>
       <c r="B20" t="n">
-        <v>0.1446</v>
+        <v>0.2044</v>
       </c>
       <c r="C20" t="n">
-        <v>0.0847</v>
+        <v>0.1067</v>
       </c>
       <c r="D20" t="n">
-        <v>0.664</v>
+        <v>0.6087</v>
       </c>
       <c r="E20" t="n">
-        <v>0.9185</v>
+        <v>0.331</v>
       </c>
       <c r="F20" t="n">
-        <v>-0.4947</v>
-      </c>
-      <c r="G20" t="n">
-        <v>0.5889</v>
-      </c>
-      <c r="H20" t="n">
-        <v>0.1248</v>
-      </c>
-      <c r="I20" t="n">
-        <v>-0.1375</v>
+        <v>0.669</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>0.1187</v>
+        <v>0.1714</v>
       </c>
       <c r="B21" t="n">
-        <v>0.1454</v>
+        <v>0.2067</v>
       </c>
       <c r="C21" t="n">
-        <v>0.08699999999999999</v>
+        <v>0.1073</v>
       </c>
       <c r="D21" t="n">
-        <v>0.6788</v>
+        <v>0.6115</v>
       </c>
       <c r="E21" t="n">
-        <v>0.9603</v>
+        <v>0.3876</v>
       </c>
       <c r="F21" t="n">
-        <v>-0.5336</v>
-      </c>
-      <c r="G21" t="n">
-        <v>0.602</v>
-      </c>
-      <c r="H21" t="n">
-        <v>0.1041</v>
-      </c>
-      <c r="I21" t="n">
-        <v>-0.1327</v>
+        <v>0.6124000000000001</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>0.1216</v>
+        <v>0.1736</v>
       </c>
       <c r="B22" t="n">
-        <v>0.1464</v>
+        <v>0.211</v>
       </c>
       <c r="C22" t="n">
-        <v>0.08939999999999999</v>
+        <v>0.1069</v>
       </c>
       <c r="D22" t="n">
-        <v>0.694</v>
+        <v>0.6098</v>
       </c>
       <c r="E22" t="n">
-        <v>1.0051</v>
+        <v>0.4497</v>
       </c>
       <c r="F22" t="n">
-        <v>-0.5755</v>
-      </c>
-      <c r="G22" t="n">
-        <v>0.6161</v>
-      </c>
-      <c r="H22" t="n">
-        <v>0.0819</v>
-      </c>
-      <c r="I22" t="n">
-        <v>-0.1276</v>
+        <v>0.5503</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>0.1247</v>
+        <v>0.1761</v>
       </c>
       <c r="B23" t="n">
-        <v>0.1476</v>
+        <v>0.2174</v>
       </c>
       <c r="C23" t="n">
-        <v>0.092</v>
+        <v>0.1052</v>
       </c>
       <c r="D23" t="n">
-        <v>0.7091</v>
+        <v>0.603</v>
       </c>
       <c r="E23" t="n">
-        <v>1.0531</v>
+        <v>0.5173</v>
       </c>
       <c r="F23" t="n">
-        <v>-0.6202</v>
-      </c>
-      <c r="G23" t="n">
-        <v>0.6311</v>
-      </c>
-      <c r="H23" t="n">
-        <v>0.0581</v>
-      </c>
-      <c r="I23" t="n">
-        <v>-0.1221</v>
+        <v>0.4827</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>0.1279</v>
+        <v>0.1787</v>
       </c>
       <c r="B24" t="n">
-        <v>0.1491</v>
+        <v>0.2262</v>
       </c>
       <c r="C24" t="n">
-        <v>0.0946</v>
+        <v>0.1019</v>
       </c>
       <c r="D24" t="n">
-        <v>0.7241</v>
+        <v>0.5911</v>
       </c>
       <c r="E24" t="n">
-        <v>1.1043</v>
+        <v>0.5906</v>
       </c>
       <c r="F24" t="n">
-        <v>-0.6679</v>
-      </c>
-      <c r="G24" t="n">
-        <v>0.6471</v>
-      </c>
-      <c r="H24" t="n">
-        <v>0.0327</v>
-      </c>
-      <c r="I24" t="n">
-        <v>-0.1163</v>
+        <v>0.4094</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>0.1314</v>
+        <v>0.1815</v>
       </c>
       <c r="B25" t="n">
-        <v>0.1508</v>
+        <v>0.2377</v>
       </c>
       <c r="C25" t="n">
-        <v>0.0973</v>
+        <v>0.0968</v>
       </c>
       <c r="D25" t="n">
-        <v>0.7388</v>
+        <v>0.5744</v>
       </c>
       <c r="E25" t="n">
-        <v>1.1585</v>
+        <v>0.6694</v>
       </c>
       <c r="F25" t="n">
-        <v>-0.7184</v>
-      </c>
-      <c r="G25" t="n">
-        <v>0.6641</v>
-      </c>
-      <c r="H25" t="n">
-        <v>0.0059</v>
-      </c>
-      <c r="I25" t="n">
-        <v>-0.1101</v>
+        <v>0.3306</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>0.1351</v>
+        <v>0.1846</v>
       </c>
       <c r="B26" t="n">
-        <v>0.1529</v>
+        <v>0.252</v>
       </c>
       <c r="C26" t="n">
-        <v>0.1</v>
+        <v>0.0893</v>
       </c>
       <c r="D26" t="n">
-        <v>0.7528</v>
+        <v>0.5538</v>
       </c>
       <c r="E26" t="n">
-        <v>1.2159</v>
+        <v>0.7538</v>
       </c>
       <c r="F26" t="n">
-        <v>-0.7719</v>
-      </c>
-      <c r="G26" t="n">
-        <v>0.6821</v>
-      </c>
-      <c r="H26" t="n">
-        <v>-0.0226</v>
-      </c>
-      <c r="I26" t="n">
-        <v>-0.1035</v>
+        <v>0.2462</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>0.139</v>
+        <v>0.1878</v>
       </c>
       <c r="B27" t="n">
-        <v>0.1553</v>
+        <v>0.2691</v>
       </c>
       <c r="C27" t="n">
-        <v>0.1028</v>
+        <v>0.0791</v>
       </c>
       <c r="D27" t="n">
-        <v>0.7661</v>
+        <v>0.5306</v>
       </c>
       <c r="E27" t="n">
-        <v>1.2763</v>
+        <v>0.8437</v>
       </c>
       <c r="F27" t="n">
-        <v>-0.8282</v>
-      </c>
-      <c r="G27" t="n">
-        <v>0.701</v>
-      </c>
-      <c r="H27" t="n">
-        <v>-0.0525</v>
-      </c>
-      <c r="I27" t="n">
-        <v>-0.09660000000000001</v>
+        <v>0.1563</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>0.1431</v>
+        <v>0.1912</v>
       </c>
       <c r="B28" t="n">
-        <v>0.1581</v>
+        <v>0.2891</v>
       </c>
       <c r="C28" t="n">
-        <v>0.1056</v>
+        <v>0.0659</v>
       </c>
       <c r="D28" t="n">
-        <v>0.7785</v>
+        <v>0.5059</v>
       </c>
       <c r="E28" t="n">
-        <v>1.3399</v>
+        <v>0.9393</v>
       </c>
       <c r="F28" t="n">
-        <v>-0.8875</v>
-      </c>
-      <c r="G28" t="n">
-        <v>0.7209</v>
-      </c>
-      <c r="H28" t="n">
-        <v>-0.08400000000000001</v>
-      </c>
-      <c r="I28" t="n">
-        <v>-0.08939999999999999</v>
+        <v>0.0607</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>0.1473</v>
+        <v>0.1948</v>
       </c>
       <c r="B29" t="n">
-        <v>0.1613</v>
+        <v>0.3117</v>
       </c>
       <c r="C29" t="n">
-        <v>0.1083</v>
+        <v>0.0491</v>
       </c>
       <c r="D29" t="n">
-        <v>0.7897</v>
+        <v>0.4807</v>
       </c>
       <c r="E29" t="n">
-        <v>1.4066</v>
+        <v>1.0404</v>
       </c>
       <c r="F29" t="n">
-        <v>-0.9497</v>
-      </c>
-      <c r="G29" t="n">
-        <v>0.7418</v>
-      </c>
-      <c r="H29" t="n">
-        <v>-0.1171</v>
-      </c>
-      <c r="I29" t="n">
-        <v>-0.08169999999999999</v>
+        <v>-0.0404</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>0.1518</v>
+        <v>0.1987</v>
       </c>
       <c r="B30" t="n">
-        <v>0.1648</v>
+        <v>0.3371</v>
       </c>
       <c r="C30" t="n">
-        <v>0.1111</v>
+        <v>0.0283</v>
       </c>
       <c r="D30" t="n">
-        <v>0.7997</v>
+        <v>0.4559</v>
       </c>
       <c r="E30" t="n">
-        <v>1.4765</v>
+        <v>1.147</v>
       </c>
       <c r="F30" t="n">
-        <v>-1.0147</v>
-      </c>
-      <c r="G30" t="n">
-        <v>0.7637</v>
-      </c>
-      <c r="H30" t="n">
-        <v>-0.1517</v>
-      </c>
-      <c r="I30" t="n">
-        <v>-0.0738</v>
+        <v>-0.147</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>0.1565</v>
+        <v>0.2027</v>
       </c>
       <c r="B31" t="n">
-        <v>0.1688</v>
+        <v>0.365</v>
       </c>
       <c r="C31" t="n">
-        <v>0.1137</v>
+        <v>0.0029</v>
       </c>
       <c r="D31" t="n">
-        <v>0.8085</v>
+        <v>0.4321</v>
       </c>
       <c r="E31" t="n">
-        <v>1.5494</v>
+        <v>1.2593</v>
       </c>
       <c r="F31" t="n">
-        <v>-1.0827</v>
-      </c>
-      <c r="G31" t="n">
-        <v>0.7866</v>
-      </c>
-      <c r="H31" t="n">
-        <v>-0.1878</v>
-      </c>
-      <c r="I31" t="n">
-        <v>-0.0654</v>
+        <v>-0.2593</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="n">
-        <v>0.1614</v>
+        <v>0.2069</v>
       </c>
       <c r="B32" t="n">
-        <v>0.1733</v>
+        <v>0.3953</v>
       </c>
       <c r="C32" t="n">
-        <v>0.1163</v>
+        <v>-0.0275</v>
       </c>
       <c r="D32" t="n">
-        <v>0.8159</v>
+        <v>0.4096</v>
       </c>
       <c r="E32" t="n">
-        <v>1.6255</v>
+        <v>1.3771</v>
       </c>
       <c r="F32" t="n">
-        <v>-1.1536</v>
-      </c>
-      <c r="G32" t="n">
-        <v>0.8104</v>
-      </c>
-      <c r="H32" t="n">
-        <v>-0.2255</v>
-      </c>
-      <c r="I32" t="n">
-        <v>-0.0568</v>
+        <v>-0.3771</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="n">
-        <v>0.1665</v>
+        <v>0.2114</v>
       </c>
       <c r="B33" t="n">
-        <v>0.1782</v>
+        <v>0.428</v>
       </c>
       <c r="C33" t="n">
-        <v>0.1188</v>
+        <v>-0.0634</v>
       </c>
       <c r="D33" t="n">
-        <v>0.822</v>
+        <v>0.3887</v>
       </c>
       <c r="E33" t="n">
-        <v>1.7046</v>
+        <v>1.5005</v>
       </c>
       <c r="F33" t="n">
-        <v>-1.2274</v>
-      </c>
-      <c r="G33" t="n">
-        <v>0.8352000000000001</v>
-      </c>
-      <c r="H33" t="n">
-        <v>-0.2647</v>
-      </c>
-      <c r="I33" t="n">
-        <v>-0.0477</v>
+        <v>-0.5004999999999999</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="n">
-        <v>0.1717</v>
+        <v>0.216</v>
       </c>
       <c r="B34" t="n">
-        <v>0.1835</v>
+        <v>0.463</v>
       </c>
       <c r="C34" t="n">
-        <v>0.1212</v>
+        <v>-0.1056</v>
       </c>
       <c r="D34" t="n">
-        <v>0.8268</v>
+        <v>0.3693</v>
       </c>
       <c r="E34" t="n">
-        <v>1.7869</v>
+        <v>1.6294</v>
       </c>
       <c r="F34" t="n">
-        <v>-1.3041</v>
-      </c>
-      <c r="G34" t="n">
-        <v>0.861</v>
-      </c>
-      <c r="H34" t="n">
-        <v>-0.3055</v>
-      </c>
-      <c r="I34" t="n">
-        <v>-0.0383</v>
+        <v>-0.6294</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="n">
-        <v>0.1772</v>
+        <v>0.2208</v>
       </c>
       <c r="B35" t="n">
-        <v>0.1894</v>
+        <v>0.5002</v>
       </c>
       <c r="C35" t="n">
-        <v>0.1234</v>
+        <v>-0.1545</v>
       </c>
       <c r="D35" t="n">
-        <v>0.8303</v>
+        <v>0.3515</v>
       </c>
       <c r="E35" t="n">
-        <v>1.8724</v>
+        <v>1.764</v>
       </c>
       <c r="F35" t="n">
-        <v>-1.3837</v>
-      </c>
-      <c r="G35" t="n">
-        <v>0.8877</v>
-      </c>
-      <c r="H35" t="n">
-        <v>-0.3478</v>
-      </c>
-      <c r="I35" t="n">
-        <v>-0.0286</v>
+        <v>-0.764</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="n">
-        <v>0.1829</v>
+        <v>0.2259</v>
       </c>
       <c r="B36" t="n">
-        <v>0.1957</v>
+        <v>0.5396</v>
       </c>
       <c r="C36" t="n">
-        <v>0.1255</v>
+        <v>-0.2108</v>
       </c>
       <c r="D36" t="n">
-        <v>0.8326</v>
+        <v>0.3352</v>
       </c>
       <c r="E36" t="n">
-        <v>1.9609</v>
+        <v>1.9041</v>
       </c>
       <c r="F36" t="n">
-        <v>-1.4662</v>
-      </c>
-      <c r="G36" t="n">
-        <v>0.9154</v>
-      </c>
-      <c r="H36" t="n">
-        <v>-0.3917</v>
-      </c>
-      <c r="I36" t="n">
-        <v>-0.0184</v>
+        <v>-0.9041</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="n">
-        <v>0.1888</v>
+        <v>0.2311</v>
       </c>
       <c r="B37" t="n">
-        <v>0.2024</v>
+        <v>0.581</v>
       </c>
       <c r="C37" t="n">
-        <v>0.1273</v>
+        <v>-0.2752</v>
       </c>
       <c r="D37" t="n">
-        <v>0.8338</v>
+        <v>0.3203</v>
       </c>
       <c r="E37" t="n">
-        <v>2.0525</v>
+        <v>2.0497</v>
       </c>
       <c r="F37" t="n">
-        <v>-1.5516</v>
-      </c>
-      <c r="G37" t="n">
-        <v>0.9442</v>
-      </c>
-      <c r="H37" t="n">
-        <v>-0.4371</v>
-      </c>
-      <c r="I37" t="n">
-        <v>-0.008</v>
+        <v>-1.0497</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="n">
-        <v>0.1949</v>
+        <v>0.2365</v>
       </c>
       <c r="B38" t="n">
-        <v>0.2097</v>
+        <v>0.6244</v>
       </c>
       <c r="C38" t="n">
-        <v>0.1289</v>
+        <v>-0.3483</v>
       </c>
       <c r="D38" t="n">
-        <v>0.834</v>
+        <v>0.3067</v>
       </c>
       <c r="E38" t="n">
-        <v>2.1473</v>
+        <v>2.201</v>
       </c>
       <c r="F38" t="n">
-        <v>-1.6399</v>
-      </c>
-      <c r="G38" t="n">
-        <v>0.9738</v>
-      </c>
-      <c r="H38" t="n">
-        <v>-0.484</v>
-      </c>
-      <c r="I38" t="n">
-        <v>0.0028</v>
+        <v>-1.201</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="n">
-        <v>0.2012</v>
+        <v>0.2421</v>
       </c>
       <c r="B39" t="n">
-        <v>0.2174</v>
+        <v>0.6698</v>
       </c>
       <c r="C39" t="n">
-        <v>0.1303</v>
+        <v>-0.4308</v>
       </c>
       <c r="D39" t="n">
-        <v>0.8332000000000001</v>
+        <v>0.2943</v>
       </c>
       <c r="E39" t="n">
-        <v>2.2452</v>
+        <v>2.3578</v>
       </c>
       <c r="F39" t="n">
-        <v>-1.7312</v>
-      </c>
-      <c r="G39" t="n">
-        <v>1.0045</v>
-      </c>
-      <c r="H39" t="n">
-        <v>-0.5325</v>
-      </c>
-      <c r="I39" t="n">
-        <v>0.014</v>
+        <v>-1.3578</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="n">
-        <v>0.2076</v>
+        <v>0.248</v>
       </c>
       <c r="B40" t="n">
-        <v>0.2256</v>
+        <v>0.7171999999999999</v>
       </c>
       <c r="C40" t="n">
-        <v>0.1313</v>
+        <v>-0.5235</v>
       </c>
       <c r="D40" t="n">
-        <v>0.8317</v>
+        <v>0.283</v>
       </c>
       <c r="E40" t="n">
-        <v>2.3462</v>
+        <v>2.5201</v>
       </c>
       <c r="F40" t="n">
-        <v>-1.8253</v>
-      </c>
-      <c r="G40" t="n">
-        <v>1.0361</v>
-      </c>
-      <c r="H40" t="n">
-        <v>-0.5826</v>
-      </c>
-      <c r="I40" t="n">
-        <v>0.0256</v>
+        <v>-1.5201</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="n">
-        <v>0.2143</v>
+        <v>0.254</v>
       </c>
       <c r="B41" t="n">
-        <v>0.2343</v>
+        <v>0.7665</v>
       </c>
       <c r="C41" t="n">
-        <v>0.132</v>
+        <v>-0.6272</v>
       </c>
       <c r="D41" t="n">
-        <v>0.8295</v>
+        <v>0.2727</v>
       </c>
       <c r="E41" t="n">
-        <v>2.4503</v>
+        <v>2.6881</v>
       </c>
       <c r="F41" t="n">
-        <v>-1.9223</v>
-      </c>
-      <c r="G41" t="n">
-        <v>1.0687</v>
-      </c>
-      <c r="H41" t="n">
-        <v>-0.6341</v>
-      </c>
-      <c r="I41" t="n">
-        <v>0.0374</v>
+        <v>-1.6881</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="n">
-        <v>0.2212</v>
+        <v>0.2602</v>
       </c>
       <c r="B42" t="n">
-        <v>0.2434</v>
+        <v>0.8176</v>
       </c>
       <c r="C42" t="n">
-        <v>0.1323</v>
+        <v>-0.7425</v>
       </c>
       <c r="D42" t="n">
-        <v>0.8267</v>
+        <v>0.2632</v>
       </c>
       <c r="E42" t="n">
-        <v>2.5575</v>
+        <v>2.8616</v>
       </c>
       <c r="F42" t="n">
-        <v>-2.0223</v>
-      </c>
-      <c r="G42" t="n">
-        <v>1.1023</v>
-      </c>
-      <c r="H42" t="n">
-        <v>-0.6873</v>
-      </c>
-      <c r="I42" t="n">
-        <v>0.0497</v>
+        <v>-1.8616</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="n">
-        <v>0.2283</v>
+        <v>0.2667</v>
       </c>
       <c r="B43" t="n">
-        <v>0.2529</v>
+        <v>0.8707</v>
       </c>
       <c r="C43" t="n">
-        <v>0.1323</v>
+        <v>-0.8704</v>
       </c>
       <c r="D43" t="n">
-        <v>0.8234</v>
+        <v>0.2546</v>
       </c>
       <c r="E43" t="n">
-        <v>2.6679</v>
+        <v>3.0407</v>
       </c>
       <c r="F43" t="n">
-        <v>-2.1251</v>
-      </c>
-      <c r="G43" t="n">
-        <v>1.1369</v>
-      </c>
-      <c r="H43" t="n">
-        <v>-0.7419</v>
-      </c>
-      <c r="I43" t="n">
-        <v>0.0623</v>
+        <v>-2.0407</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="n">
-        <v>0.2356</v>
+        <v>0.2733</v>
       </c>
       <c r="B44" t="n">
-        <v>0.263</v>
+        <v>0.9255</v>
       </c>
       <c r="C44" t="n">
-        <v>0.1318</v>
+        <v>-1.0116</v>
       </c>
       <c r="D44" t="n">
-        <v>0.8197</v>
+        <v>0.2467</v>
       </c>
       <c r="E44" t="n">
-        <v>2.7813</v>
+        <v>3.2254</v>
       </c>
       <c r="F44" t="n">
-        <v>-2.2309</v>
-      </c>
-      <c r="G44" t="n">
-        <v>1.1724</v>
-      </c>
-      <c r="H44" t="n">
-        <v>-0.7982</v>
-      </c>
-      <c r="I44" t="n">
-        <v>0.07530000000000001</v>
+        <v>-2.2254</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="n">
-        <v>0.243</v>
+        <v>0.2801</v>
       </c>
       <c r="B45" t="n">
-        <v>0.2734</v>
+        <v>0.9822</v>
       </c>
       <c r="C45" t="n">
-        <v>0.1309</v>
+        <v>-1.1671</v>
       </c>
       <c r="D45" t="n">
-        <v>0.8156</v>
+        <v>0.2394</v>
       </c>
       <c r="E45" t="n">
-        <v>2.8979</v>
+        <v>3.4156</v>
       </c>
       <c r="F45" t="n">
-        <v>-2.3395</v>
-      </c>
-      <c r="G45" t="n">
-        <v>1.209</v>
-      </c>
-      <c r="H45" t="n">
-        <v>-0.8559</v>
-      </c>
-      <c r="I45" t="n">
-        <v>0.0886</v>
+        <v>-2.4156</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="n">
-        <v>0.2507</v>
+        <v>0.2872</v>
       </c>
       <c r="B46" t="n">
-        <v>0.2844</v>
+        <v>1.0408</v>
       </c>
       <c r="C46" t="n">
-        <v>0.1294</v>
+        <v>-1.3376</v>
       </c>
       <c r="D46" t="n">
-        <v>0.8114</v>
+        <v>0.2327</v>
       </c>
       <c r="E46" t="n">
-        <v>3.0176</v>
+        <v>3.6114</v>
       </c>
       <c r="F46" t="n">
-        <v>-2.4511</v>
-      </c>
-      <c r="G46" t="n">
-        <v>1.2464</v>
-      </c>
-      <c r="H46" t="n">
-        <v>-0.9152</v>
-      </c>
-      <c r="I46" t="n">
-        <v>0.1022</v>
+        <v>-2.6114</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="n">
-        <v>0.2586</v>
+        <v>0.2944</v>
       </c>
       <c r="B47" t="n">
-        <v>0.2957</v>
+        <v>1.1011</v>
       </c>
       <c r="C47" t="n">
-        <v>0.1274</v>
+        <v>-1.5242</v>
       </c>
       <c r="D47" t="n">
-        <v>0.8069</v>
+        <v>0.2265</v>
       </c>
       <c r="E47" t="n">
-        <v>3.1404</v>
+        <v>3.8128</v>
       </c>
       <c r="F47" t="n">
-        <v>-2.5655</v>
-      </c>
-      <c r="G47" t="n">
-        <v>1.2849</v>
-      </c>
-      <c r="H47" t="n">
-        <v>-0.9761</v>
-      </c>
-      <c r="I47" t="n">
-        <v>0.1163</v>
+        <v>-2.8128</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="n">
-        <v>0.2667</v>
+        <v>0.3018</v>
       </c>
       <c r="B48" t="n">
-        <v>0.3075</v>
+        <v>1.1632</v>
       </c>
       <c r="C48" t="n">
-        <v>0.1249</v>
+        <v>-1.7277</v>
       </c>
       <c r="D48" t="n">
-        <v>0.8023</v>
+        <v>0.2208</v>
       </c>
       <c r="E48" t="n">
-        <v>3.2664</v>
+        <v>4.0198</v>
       </c>
       <c r="F48" t="n">
-        <v>-2.6829</v>
-      </c>
-      <c r="G48" t="n">
-        <v>1.3244</v>
-      </c>
-      <c r="H48" t="n">
-        <v>-1.0385</v>
-      </c>
-      <c r="I48" t="n">
-        <v>0.1306</v>
+        <v>-3.0198</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="n">
-        <v>0.275</v>
+        <v>0.3094</v>
       </c>
       <c r="B49" t="n">
-        <v>0.3197</v>
+        <v>1.2271</v>
       </c>
       <c r="C49" t="n">
-        <v>0.1217</v>
+        <v>-1.9492</v>
       </c>
       <c r="D49" t="n">
-        <v>0.7976</v>
+        <v>0.2155</v>
       </c>
       <c r="E49" t="n">
-        <v>3.3954</v>
+        <v>4.2323</v>
       </c>
       <c r="F49" t="n">
-        <v>-2.8032</v>
-      </c>
-      <c r="G49" t="n">
-        <v>1.3648</v>
-      </c>
-      <c r="H49" t="n">
-        <v>-1.1024</v>
-      </c>
-      <c r="I49" t="n">
-        <v>0.1454</v>
+        <v>-3.2323</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="n">
-        <v>0.2834</v>
+        <v>0.3173</v>
       </c>
       <c r="B50" t="n">
-        <v>0.3323</v>
+        <v>1.2928</v>
       </c>
       <c r="C50" t="n">
-        <v>0.1178</v>
+        <v>-2.1896</v>
       </c>
       <c r="D50" t="n">
-        <v>0.7929</v>
+        <v>0.2106</v>
       </c>
       <c r="E50" t="n">
-        <v>3.5276</v>
+        <v>4.4504</v>
       </c>
       <c r="F50" t="n">
-        <v>-2.9264</v>
-      </c>
-      <c r="G50" t="n">
-        <v>1.4062</v>
-      </c>
-      <c r="H50" t="n">
-        <v>-1.1679</v>
-      </c>
-      <c r="I50" t="n">
-        <v>0.1605</v>
+        <v>-3.4504</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="n">
-        <v>0.2921</v>
+        <v>0.3253</v>
       </c>
       <c r="B51" t="n">
-        <v>0.3453</v>
+        <v>1.3602</v>
       </c>
       <c r="C51" t="n">
-        <v>0.1133</v>
+        <v>-2.4499</v>
       </c>
       <c r="D51" t="n">
-        <v>0.7881</v>
+        <v>0.2061</v>
       </c>
       <c r="E51" t="n">
-        <v>3.6629</v>
+        <v>4.674</v>
       </c>
       <c r="F51" t="n">
-        <v>-3.0524</v>
-      </c>
-      <c r="G51" t="n">
-        <v>1.4486</v>
-      </c>
-      <c r="H51" t="n">
-        <v>-1.2349</v>
-      </c>
-      <c r="I51" t="n">
-        <v>0.1759</v>
+        <v>-3.674</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="n">
-        <v>0.301</v>
+        <v>0.3335</v>
       </c>
       <c r="B52" t="n">
-        <v>0.3587</v>
+        <v>1.4294</v>
       </c>
       <c r="C52" t="n">
-        <v>0.108</v>
+        <v>-2.7312</v>
       </c>
       <c r="D52" t="n">
-        <v>0.7834</v>
+        <v>0.2019</v>
       </c>
       <c r="E52" t="n">
-        <v>3.8013</v>
+        <v>4.9033</v>
       </c>
       <c r="F52" t="n">
-        <v>-3.1814</v>
-      </c>
-      <c r="G52" t="n">
-        <v>1.4919</v>
-      </c>
-      <c r="H52" t="n">
-        <v>-1.3035</v>
-      </c>
-      <c r="I52" t="n">
-        <v>0.1917</v>
+        <v>-3.9033</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="n">
-        <v>0.3101</v>
+        <v>0.342</v>
       </c>
       <c r="B53" t="n">
-        <v>0.3725</v>
+        <v>1.5003</v>
       </c>
       <c r="C53" t="n">
-        <v>0.1019</v>
+        <v>-3.0346</v>
       </c>
       <c r="D53" t="n">
-        <v>0.7786999999999999</v>
+        <v>0.1979</v>
       </c>
       <c r="E53" t="n">
-        <v>3.9428</v>
+        <v>5.1381</v>
       </c>
       <c r="F53" t="n">
-        <v>-3.3133</v>
-      </c>
-      <c r="G53" t="n">
-        <v>1.5362</v>
-      </c>
-      <c r="H53" t="n">
-        <v>-1.3736</v>
-      </c>
-      <c r="I53" t="n">
-        <v>0.2079</v>
+        <v>-4.1381</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="n">
-        <v>0.3194</v>
+        <v>0.3506</v>
       </c>
       <c r="B54" t="n">
-        <v>0.3867</v>
+        <v>1.573</v>
       </c>
       <c r="C54" t="n">
-        <v>0.095</v>
+        <v>-3.3611</v>
       </c>
       <c r="D54" t="n">
-        <v>0.7741</v>
+        <v>0.1943</v>
       </c>
       <c r="E54" t="n">
-        <v>4.0874</v>
+        <v>5.3784</v>
       </c>
       <c r="F54" t="n">
-        <v>-3.4481</v>
-      </c>
-      <c r="G54" t="n">
-        <v>1.5815</v>
-      </c>
-      <c r="H54" t="n">
-        <v>-1.4453</v>
-      </c>
-      <c r="I54" t="n">
-        <v>0.2244</v>
+        <v>-4.3784</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="n">
-        <v>0.3288</v>
+        <v>0.3594</v>
       </c>
       <c r="B55" t="n">
-        <v>0.4013</v>
+        <v>1.6475</v>
       </c>
       <c r="C55" t="n">
-        <v>0.0872</v>
+        <v>-3.7119</v>
       </c>
       <c r="D55" t="n">
-        <v>0.7695</v>
+        <v>0.1908</v>
       </c>
       <c r="E55" t="n">
-        <v>4.2352</v>
+        <v>5.6244</v>
       </c>
       <c r="F55" t="n">
-        <v>-3.5858</v>
-      </c>
-      <c r="G55" t="n">
-        <v>1.6278</v>
-      </c>
-      <c r="H55" t="n">
-        <v>-1.5185</v>
-      </c>
-      <c r="I55" t="n">
-        <v>0.2413</v>
+        <v>-4.6244</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="n">
-        <v>0.3385</v>
+        <v>0.3684</v>
       </c>
       <c r="B56" t="n">
-        <v>0.4163</v>
+        <v>1.7237</v>
       </c>
       <c r="C56" t="n">
-        <v>0.0785</v>
+        <v>-4.0881</v>
       </c>
       <c r="D56" t="n">
-        <v>0.765</v>
+        <v>0.1877</v>
       </c>
       <c r="E56" t="n">
-        <v>4.3861</v>
+        <v>5.8759</v>
       </c>
       <c r="F56" t="n">
-        <v>-3.7264</v>
-      </c>
-      <c r="G56" t="n">
-        <v>1.6751</v>
-      </c>
-      <c r="H56" t="n">
-        <v>-1.5932</v>
-      </c>
-      <c r="I56" t="n">
-        <v>0.2585</v>
+        <v>-4.8759</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="n">
-        <v>0.3484</v>
+        <v>0.3777</v>
       </c>
       <c r="B57" t="n">
-        <v>0.4317</v>
+        <v>1.8016</v>
       </c>
       <c r="C57" t="n">
-        <v>0.0688</v>
+        <v>-4.4908</v>
       </c>
       <c r="D57" t="n">
-        <v>0.7607</v>
+        <v>0.1847</v>
       </c>
       <c r="E57" t="n">
-        <v>4.54</v>
+        <v>6.133</v>
       </c>
       <c r="F57" t="n">
-        <v>-3.87</v>
-      </c>
-      <c r="G57" t="n">
-        <v>1.7233</v>
-      </c>
-      <c r="H57" t="n">
-        <v>-1.6695</v>
-      </c>
-      <c r="I57" t="n">
-        <v>0.2761</v>
+        <v>-5.133</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="n">
-        <v>0.3585</v>
+        <v>0.3871</v>
       </c>
       <c r="B58" t="n">
-        <v>0.4475</v>
+        <v>1.8812</v>
       </c>
       <c r="C58" t="n">
-        <v>0.0581</v>
+        <v>-4.9214</v>
       </c>
       <c r="D58" t="n">
-        <v>0.7564</v>
+        <v>0.1819</v>
       </c>
       <c r="E58" t="n">
-        <v>4.6971</v>
+        <v>6.3956</v>
       </c>
       <c r="F58" t="n">
-        <v>-4.0164</v>
-      </c>
-      <c r="G58" t="n">
-        <v>1.7725</v>
-      </c>
-      <c r="H58" t="n">
-        <v>-1.7474</v>
-      </c>
-      <c r="I58" t="n">
-        <v>0.2941</v>
+        <v>-5.3956</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="n">
-        <v>0.3688</v>
+        <v>0.3967</v>
       </c>
       <c r="B59" t="n">
-        <v>0.4636</v>
+        <v>1.9626</v>
       </c>
       <c r="C59" t="n">
-        <v>0.0463</v>
+        <v>-5.381</v>
       </c>
       <c r="D59" t="n">
-        <v>0.7522</v>
+        <v>0.1792</v>
       </c>
       <c r="E59" t="n">
-        <v>4.8574</v>
+        <v>6.6639</v>
       </c>
       <c r="F59" t="n">
-        <v>-4.1657</v>
-      </c>
-      <c r="G59" t="n">
-        <v>1.8227</v>
-      </c>
-      <c r="H59" t="n">
-        <v>-1.8267</v>
-      </c>
-      <c r="I59" t="n">
-        <v>0.3124</v>
+        <v>-5.6639</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="n">
-        <v>0.3792</v>
+        <v>0.4066</v>
       </c>
       <c r="B60" t="n">
-        <v>0.4801</v>
+        <v>2.0457</v>
       </c>
       <c r="C60" t="n">
-        <v>0.0334</v>
+        <v>-5.8709</v>
       </c>
       <c r="D60" t="n">
-        <v>0.7482</v>
+        <v>0.1767</v>
       </c>
       <c r="E60" t="n">
-        <v>5.0207</v>
+        <v>6.9377</v>
       </c>
       <c r="F60" t="n">
-        <v>-4.3179</v>
-      </c>
-      <c r="G60" t="n">
-        <v>1.8739</v>
-      </c>
-      <c r="H60" t="n">
-        <v>-1.9077</v>
-      </c>
-      <c r="I60" t="n">
-        <v>0.331</v>
+        <v>-5.9377</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="n">
-        <v>0.3899</v>
+        <v>0.4166</v>
       </c>
       <c r="B61" t="n">
-        <v>0.497</v>
+        <v>2.1305</v>
       </c>
       <c r="C61" t="n">
-        <v>0.0193</v>
+        <v>-6.3923</v>
       </c>
       <c r="D61" t="n">
-        <v>0.7442</v>
+        <v>0.1744</v>
       </c>
       <c r="E61" t="n">
-        <v>5.1872</v>
+        <v>7.217</v>
       </c>
       <c r="F61" t="n">
-        <v>-4.4731</v>
-      </c>
-      <c r="G61" t="n">
-        <v>1.926</v>
-      </c>
-      <c r="H61" t="n">
-        <v>-1.9901</v>
-      </c>
-      <c r="I61" t="n">
-        <v>0.35</v>
+        <v>-6.217</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="n">
-        <v>0.4008</v>
+        <v>0.4268</v>
       </c>
       <c r="B62" t="n">
-        <v>0.5143</v>
+        <v>2.2171</v>
       </c>
       <c r="C62" t="n">
-        <v>0.004</v>
+        <v>-6.9465</v>
       </c>
       <c r="D62" t="n">
-        <v>0.7403999999999999</v>
+        <v>0.1722</v>
       </c>
       <c r="E62" t="n">
-        <v>5.3567</v>
+        <v>7.502</v>
       </c>
       <c r="F62" t="n">
-        <v>-4.6311</v>
-      </c>
-      <c r="G62" t="n">
-        <v>1.9791</v>
-      </c>
-      <c r="H62" t="n">
-        <v>-2.0741</v>
-      </c>
-      <c r="I62" t="n">
-        <v>0.3694</v>
+        <v>-6.502</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="n">
-        <v>0.4119</v>
+        <v>0.4373</v>
       </c>
       <c r="B63" t="n">
-        <v>0.5319</v>
+        <v>2.3054</v>
       </c>
       <c r="C63" t="n">
-        <v>-0.0125</v>
+        <v>-7.535</v>
       </c>
       <c r="D63" t="n">
-        <v>0.7367</v>
+        <v>0.1701</v>
       </c>
       <c r="E63" t="n">
-        <v>5.5294</v>
+        <v>7.7925</v>
       </c>
       <c r="F63" t="n">
-        <v>-4.7921</v>
-      </c>
-      <c r="G63" t="n">
-        <v>2.0332</v>
-      </c>
-      <c r="H63" t="n">
-        <v>-2.1597</v>
-      </c>
-      <c r="I63" t="n">
-        <v>0.3891</v>
+        <v>-6.7925</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="n">
-        <v>0.4232</v>
+        <v>0.4479</v>
       </c>
       <c r="B64" t="n">
-        <v>0.5499000000000001</v>
+        <v>2.3954</v>
       </c>
       <c r="C64" t="n">
-        <v>-0.0305</v>
+        <v>-8.158899999999999</v>
       </c>
       <c r="D64" t="n">
-        <v>0.7331</v>
+        <v>0.1682</v>
       </c>
       <c r="E64" t="n">
-        <v>5.7052</v>
+        <v>8.0886</v>
       </c>
       <c r="F64" t="n">
-        <v>-4.9559</v>
-      </c>
-      <c r="G64" t="n">
-        <v>2.0883</v>
-      </c>
-      <c r="H64" t="n">
-        <v>-2.2468</v>
-      </c>
-      <c r="I64" t="n">
-        <v>0.4092</v>
+        <v>-7.0886</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="n">
-        <v>0.4346</v>
+        <v>0.4587</v>
       </c>
       <c r="B65" t="n">
-        <v>0.5683</v>
+        <v>2.4871</v>
       </c>
       <c r="C65" t="n">
-        <v>-0.0498</v>
+        <v>-8.819800000000001</v>
       </c>
       <c r="D65" t="n">
-        <v>0.7296</v>
+        <v>0.1663</v>
       </c>
       <c r="E65" t="n">
-        <v>5.8842</v>
+        <v>8.3902</v>
       </c>
       <c r="F65" t="n">
-        <v>-5.1227</v>
-      </c>
-      <c r="G65" t="n">
-        <v>2.1443</v>
-      </c>
-      <c r="H65" t="n">
-        <v>-2.3355</v>
-      </c>
-      <c r="I65" t="n">
-        <v>0.4296</v>
+        <v>-7.3902</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="n">
-        <v>0.4463</v>
+        <v>0.4697</v>
       </c>
       <c r="B66" t="n">
-        <v>0.587</v>
+        <v>2.5805</v>
       </c>
       <c r="C66" t="n">
-        <v>-0.07049999999999999</v>
+        <v>-9.5191</v>
       </c>
       <c r="D66" t="n">
-        <v>0.7262999999999999</v>
+        <v>0.1646</v>
       </c>
       <c r="E66" t="n">
-        <v>6.0662</v>
+        <v>8.6975</v>
       </c>
       <c r="F66" t="n">
-        <v>-5.2923</v>
-      </c>
-      <c r="G66" t="n">
-        <v>2.2014</v>
-      </c>
-      <c r="H66" t="n">
-        <v>-2.4256</v>
-      </c>
-      <c r="I66" t="n">
-        <v>0.4504</v>
+        <v>-7.6975</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="n">
-        <v>0.4582</v>
+        <v>0.481</v>
       </c>
       <c r="B67" t="n">
-        <v>0.6061</v>
+        <v>2.6757</v>
       </c>
       <c r="C67" t="n">
-        <v>-0.09279999999999999</v>
+        <v>-10.2581</v>
       </c>
       <c r="D67" t="n">
-        <v>0.723</v>
+        <v>0.1629</v>
       </c>
       <c r="E67" t="n">
-        <v>6.2514</v>
+        <v>9.010300000000001</v>
       </c>
       <c r="F67" t="n">
-        <v>-5.4649</v>
-      </c>
-      <c r="G67" t="n">
-        <v>2.2594</v>
-      </c>
-      <c r="H67" t="n">
-        <v>-2.5174</v>
-      </c>
-      <c r="I67" t="n">
-        <v>0.4716</v>
+        <v>-8.010300000000001</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="n">
-        <v>0.4703</v>
+        <v>0.4924</v>
       </c>
       <c r="B68" t="n">
-        <v>0.6254999999999999</v>
+        <v>2.7726</v>
       </c>
       <c r="C68" t="n">
-        <v>-0.1166</v>
+        <v>-11.0383</v>
       </c>
       <c r="D68" t="n">
-        <v>0.7199</v>
+        <v>0.1614</v>
       </c>
       <c r="E68" t="n">
-        <v>6.4396</v>
+        <v>9.3286</v>
       </c>
       <c r="F68" t="n">
-        <v>-5.6404</v>
-      </c>
-      <c r="G68" t="n">
-        <v>2.3183</v>
-      </c>
-      <c r="H68" t="n">
-        <v>-2.6107</v>
-      </c>
-      <c r="I68" t="n">
-        <v>0.4931</v>
+        <v>-8.3286</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="n">
-        <v>0.4826</v>
+        <v>0.504</v>
       </c>
       <c r="B69" t="n">
-        <v>0.6453</v>
+        <v>2.8711</v>
       </c>
       <c r="C69" t="n">
-        <v>-0.142</v>
+        <v>-11.8612</v>
       </c>
       <c r="D69" t="n">
-        <v>0.7168</v>
+        <v>0.1599</v>
       </c>
       <c r="E69" t="n">
-        <v>6.631</v>
+        <v>9.6526</v>
       </c>
       <c r="F69" t="n">
-        <v>-5.8187</v>
-      </c>
-      <c r="G69" t="n">
-        <v>2.3783</v>
-      </c>
-      <c r="H69" t="n">
-        <v>-2.7055</v>
-      </c>
-      <c r="I69" t="n">
-        <v>0.5149</v>
+        <v>-8.6526</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="n">
-        <v>0.495</v>
+        <v>0.5159</v>
       </c>
       <c r="B70" t="n">
-        <v>0.6654</v>
+        <v>2.9714</v>
       </c>
       <c r="C70" t="n">
-        <v>-0.1691</v>
+        <v>-12.7283</v>
       </c>
       <c r="D70" t="n">
-        <v>0.7139</v>
+        <v>0.1585</v>
       </c>
       <c r="E70" t="n">
-        <v>6.8255</v>
+        <v>9.982100000000001</v>
       </c>
       <c r="F70" t="n">
-        <v>-6</v>
-      </c>
-      <c r="G70" t="n">
-        <v>2.4392</v>
-      </c>
-      <c r="H70" t="n">
-        <v>-2.8019</v>
-      </c>
-      <c r="I70" t="n">
-        <v>0.5371</v>
+        <v>-8.982100000000001</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="n">
-        <v>0.5077</v>
+        <v>0.5279</v>
       </c>
       <c r="B71" t="n">
-        <v>0.6859</v>
+        <v>3.0734</v>
       </c>
       <c r="C71" t="n">
-        <v>-0.198</v>
+        <v>-13.6412</v>
       </c>
       <c r="D71" t="n">
-        <v>0.7111</v>
+        <v>0.1571</v>
       </c>
       <c r="E71" t="n">
-        <v>7.0232</v>
+        <v>10.3172</v>
       </c>
       <c r="F71" t="n">
-        <v>-6.1842</v>
-      </c>
-      <c r="G71" t="n">
-        <v>2.5011</v>
-      </c>
-      <c r="H71" t="n">
-        <v>-2.8998</v>
-      </c>
-      <c r="I71" t="n">
-        <v>0.5597</v>
+        <v>-9.3172</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="n">
-        <v>0.5206</v>
+        <v>0.5401</v>
       </c>
       <c r="B72" t="n">
-        <v>0.7067</v>
+        <v>3.1772</v>
       </c>
       <c r="C72" t="n">
-        <v>-0.2286</v>
+        <v>-14.6014</v>
       </c>
       <c r="D72" t="n">
-        <v>0.7083</v>
+        <v>0.1558</v>
       </c>
       <c r="E72" t="n">
-        <v>7.2239</v>
+        <v>10.6578</v>
       </c>
       <c r="F72" t="n">
-        <v>-6.3713</v>
-      </c>
-      <c r="G72" t="n">
-        <v>2.564</v>
-      </c>
-      <c r="H72" t="n">
-        <v>-2.9992</v>
-      </c>
-      <c r="I72" t="n">
-        <v>0.5826</v>
+        <v>-9.6578</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="n">
-        <v>0.5337</v>
+        <v>0.5525</v>
       </c>
       <c r="B73" t="n">
-        <v>0.7279</v>
+        <v>3.2826</v>
       </c>
       <c r="C73" t="n">
-        <v>-0.2612</v>
+        <v>-15.6106</v>
       </c>
       <c r="D73" t="n">
-        <v>0.7057</v>
+        <v>0.1546</v>
       </c>
       <c r="E73" t="n">
-        <v>7.4278</v>
+        <v>11.0041</v>
       </c>
       <c r="F73" t="n">
-        <v>-6.5613</v>
-      </c>
-      <c r="G73" t="n">
-        <v>2.6279</v>
-      </c>
-      <c r="H73" t="n">
-        <v>-3.1002</v>
-      </c>
-      <c r="I73" t="n">
-        <v>0.6059</v>
+        <v>-10.0041</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="n">
-        <v>0.547</v>
+        <v>0.5652</v>
       </c>
       <c r="B74" t="n">
-        <v>0.7495000000000001</v>
+        <v>3.3897</v>
       </c>
       <c r="C74" t="n">
-        <v>-0.2956</v>
+        <v>-16.6702</v>
       </c>
       <c r="D74" t="n">
-        <v>0.7030999999999999</v>
+        <v>0.1535</v>
       </c>
       <c r="E74" t="n">
-        <v>7.6348</v>
+        <v>11.3559</v>
       </c>
       <c r="F74" t="n">
-        <v>-6.7542</v>
-      </c>
-      <c r="G74" t="n">
-        <v>2.6927</v>
-      </c>
-      <c r="H74" t="n">
-        <v>-3.2028</v>
-      </c>
-      <c r="I74" t="n">
-        <v>0.6294999999999999</v>
+        <v>-10.3559</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="n">
-        <v>0.5604</v>
+        <v>0.578</v>
       </c>
       <c r="B75" t="n">
-        <v>0.7714</v>
+        <v>3.4986</v>
       </c>
       <c r="C75" t="n">
-        <v>-0.3321</v>
+        <v>-17.782</v>
       </c>
       <c r="D75" t="n">
-        <v>0.7006</v>
+        <v>0.1523</v>
       </c>
       <c r="E75" t="n">
-        <v>7.8449</v>
+        <v>11.7132</v>
       </c>
       <c r="F75" t="n">
-        <v>-6.95</v>
-      </c>
-      <c r="G75" t="n">
-        <v>2.7585</v>
-      </c>
-      <c r="H75" t="n">
-        <v>-3.3069</v>
-      </c>
-      <c r="I75" t="n">
-        <v>0.6535</v>
+        <v>-10.7132</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="n">
-        <v>0.5741000000000001</v>
+        <v>0.591</v>
       </c>
       <c r="B76" t="n">
-        <v>0.7936</v>
+        <v>3.6091</v>
       </c>
       <c r="C76" t="n">
-        <v>-0.3706</v>
+        <v>-18.9477</v>
       </c>
       <c r="D76" t="n">
-        <v>0.6982</v>
+        <v>0.1513</v>
       </c>
       <c r="E76" t="n">
-        <v>8.0581</v>
+        <v>12.0762</v>
       </c>
       <c r="F76" t="n">
-        <v>-7.1487</v>
-      </c>
-      <c r="G76" t="n">
-        <v>2.8253</v>
-      </c>
-      <c r="H76" t="n">
-        <v>-3.4125</v>
-      </c>
-      <c r="I76" t="n">
-        <v>0.6778999999999999</v>
+        <v>-11.0762</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="n">
-        <v>0.588</v>
+        <v>0.6042999999999999</v>
       </c>
       <c r="B77" t="n">
-        <v>0.8162</v>
+        <v>3.7214</v>
       </c>
       <c r="C77" t="n">
-        <v>-0.4113</v>
+        <v>-20.1689</v>
       </c>
       <c r="D77" t="n">
-        <v>0.6959</v>
+        <v>0.1503</v>
       </c>
       <c r="E77" t="n">
-        <v>8.2744</v>
+        <v>12.4447</v>
       </c>
       <c r="F77" t="n">
-        <v>-7.3503</v>
-      </c>
-      <c r="G77" t="n">
-        <v>2.893</v>
-      </c>
-      <c r="H77" t="n">
-        <v>-3.5197</v>
-      </c>
-      <c r="I77" t="n">
-        <v>0.7026</v>
+        <v>-11.4447</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="n">
-        <v>0.6021</v>
+        <v>0.6177</v>
       </c>
       <c r="B78" t="n">
-        <v>0.8391</v>
+        <v>3.8354</v>
       </c>
       <c r="C78" t="n">
-        <v>-0.4542</v>
+        <v>-21.4474</v>
       </c>
       <c r="D78" t="n">
-        <v>0.6937</v>
+        <v>0.1493</v>
       </c>
       <c r="E78" t="n">
-        <v>8.4938</v>
+        <v>12.8187</v>
       </c>
       <c r="F78" t="n">
-        <v>-7.5549</v>
-      </c>
-      <c r="G78" t="n">
-        <v>2.9618</v>
-      </c>
-      <c r="H78" t="n">
-        <v>-3.6284</v>
-      </c>
-      <c r="I78" t="n">
-        <v>0.7277</v>
+        <v>-11.8187</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="n">
-        <v>0.6163999999999999</v>
+        <v>0.6313</v>
       </c>
       <c r="B79" t="n">
-        <v>0.8624000000000001</v>
+        <v>3.951</v>
       </c>
       <c r="C79" t="n">
-        <v>-0.4993</v>
+        <v>-22.7848</v>
       </c>
       <c r="D79" t="n">
-        <v>0.6915</v>
+        <v>0.1484</v>
       </c>
       <c r="E79" t="n">
-        <v>8.7164</v>
+        <v>13.1984</v>
       </c>
       <c r="F79" t="n">
-        <v>-7.7623</v>
-      </c>
-      <c r="G79" t="n">
-        <v>3.0315</v>
-      </c>
-      <c r="H79" t="n">
-        <v>-3.7387</v>
-      </c>
-      <c r="I79" t="n">
-        <v>0.7531</v>
+        <v>-12.1984</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="n">
-        <v>0.6308</v>
+        <v>0.6452</v>
       </c>
       <c r="B80" t="n">
-        <v>0.886</v>
+        <v>4.0684</v>
       </c>
       <c r="C80" t="n">
-        <v>-0.5468</v>
+        <v>-24.183</v>
       </c>
       <c r="D80" t="n">
-        <v>0.6894</v>
+        <v>0.1475</v>
       </c>
       <c r="E80" t="n">
-        <v>8.9421</v>
+        <v>13.5836</v>
       </c>
       <c r="F80" t="n">
-        <v>-7.9726</v>
-      </c>
-      <c r="G80" t="n">
-        <v>3.1022</v>
-      </c>
-      <c r="H80" t="n">
-        <v>-3.8505</v>
-      </c>
-      <c r="I80" t="n">
-        <v>0.7789</v>
+        <v>-12.5836</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="n">
-        <v>0.6455</v>
+        <v>0.6592</v>
       </c>
       <c r="B81" t="n">
-        <v>0.91</v>
+        <v>4.1875</v>
       </c>
       <c r="C81" t="n">
-        <v>-0.5967</v>
+        <v>-25.6438</v>
       </c>
       <c r="D81" t="n">
-        <v>0.6874</v>
+        <v>0.1467</v>
       </c>
       <c r="E81" t="n">
-        <v>9.1709</v>
+        <v>13.9744</v>
       </c>
       <c r="F81" t="n">
-        <v>-8.1859</v>
-      </c>
-      <c r="G81" t="n">
-        <v>3.1739</v>
-      </c>
-      <c r="H81" t="n">
-        <v>-3.9639</v>
-      </c>
-      <c r="I81" t="n">
-        <v>0.805</v>
+        <v>-12.9744</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="n">
-        <v>0.6604</v>
+        <v>0.6734</v>
       </c>
       <c r="B82" t="n">
-        <v>0.9343</v>
+        <v>4.3083</v>
       </c>
       <c r="C82" t="n">
-        <v>-0.649</v>
+        <v>-27.169</v>
       </c>
       <c r="D82" t="n">
-        <v>0.6854</v>
+        <v>0.1459</v>
       </c>
       <c r="E82" t="n">
-        <v>9.402799999999999</v>
+        <v>14.3708</v>
       </c>
       <c r="F82" t="n">
-        <v>-8.401999999999999</v>
-      </c>
-      <c r="G82" t="n">
-        <v>3.2465</v>
-      </c>
-      <c r="H82" t="n">
-        <v>-4.0788</v>
-      </c>
-      <c r="I82" t="n">
-        <v>0.8315</v>
+        <v>-13.3708</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="n">
-        <v>0.6755</v>
+        <v>0.6878</v>
       </c>
       <c r="B83" t="n">
-        <v>0.959</v>
+        <v>4.4308</v>
       </c>
       <c r="C83" t="n">
-        <v>-0.7039</v>
+        <v>-28.7604</v>
       </c>
       <c r="D83" t="n">
-        <v>0.6835</v>
+        <v>0.1451</v>
       </c>
       <c r="E83" t="n">
-        <v>9.6378</v>
+        <v>14.7727</v>
       </c>
       <c r="F83" t="n">
-        <v>-8.6211</v>
-      </c>
-      <c r="G83" t="n">
-        <v>3.3201</v>
-      </c>
-      <c r="H83" t="n">
-        <v>-4.1952</v>
-      </c>
-      <c r="I83" t="n">
-        <v>0.8583</v>
+        <v>-13.7727</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="n">
-        <v>0.6908</v>
+        <v>0.7025</v>
       </c>
       <c r="B84" t="n">
-        <v>0.984</v>
+        <v>4.555</v>
       </c>
       <c r="C84" t="n">
-        <v>-0.7615</v>
+        <v>-30.4199</v>
       </c>
       <c r="D84" t="n">
-        <v>0.6817</v>
+        <v>0.1443</v>
       </c>
       <c r="E84" t="n">
-        <v>9.875999999999999</v>
+        <v>15.1802</v>
       </c>
       <c r="F84" t="n">
-        <v>-8.843</v>
-      </c>
-      <c r="G84" t="n">
-        <v>3.3947</v>
-      </c>
-      <c r="H84" t="n">
-        <v>-4.3132</v>
-      </c>
-      <c r="I84" t="n">
-        <v>0.8855</v>
+        <v>-14.1802</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="n">
-        <v>0.7062</v>
+        <v>0.7173</v>
       </c>
       <c r="B85" t="n">
-        <v>1.0093</v>
+        <v>4.6809</v>
       </c>
       <c r="C85" t="n">
-        <v>-0.8218</v>
+        <v>-32.1495</v>
       </c>
       <c r="D85" t="n">
-        <v>0.6798999999999999</v>
+        <v>0.1436</v>
       </c>
       <c r="E85" t="n">
-        <v>10.1173</v>
+        <v>15.5933</v>
       </c>
       <c r="F85" t="n">
-        <v>-9.0679</v>
-      </c>
-      <c r="G85" t="n">
-        <v>3.4703</v>
-      </c>
-      <c r="H85" t="n">
-        <v>-4.4327</v>
-      </c>
-      <c r="I85" t="n">
-        <v>0.9131</v>
+        <v>-14.5933</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="n">
-        <v>0.7219</v>
+        <v>0.7323</v>
       </c>
       <c r="B86" t="n">
-        <v>1.035</v>
+        <v>4.8086</v>
       </c>
       <c r="C86" t="n">
-        <v>-0.8848</v>
+        <v>-33.951</v>
       </c>
       <c r="D86" t="n">
-        <v>0.6782</v>
+        <v>0.1429</v>
       </c>
       <c r="E86" t="n">
-        <v>10.3616</v>
+        <v>16.0119</v>
       </c>
       <c r="F86" t="n">
-        <v>-9.2956</v>
-      </c>
-      <c r="G86" t="n">
-        <v>3.5468</v>
-      </c>
-      <c r="H86" t="n">
-        <v>-4.5538</v>
-      </c>
-      <c r="I86" t="n">
-        <v>0.9409999999999999</v>
+        <v>-15.0119</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="n">
-        <v>0.7378</v>
+        <v>0.7476</v>
       </c>
       <c r="B87" t="n">
-        <v>1.061</v>
+        <v>4.9379</v>
       </c>
       <c r="C87" t="n">
-        <v>-0.9507</v>
+        <v>-35.8264</v>
       </c>
       <c r="D87" t="n">
-        <v>0.6765</v>
+        <v>0.1423</v>
       </c>
       <c r="E87" t="n">
-        <v>10.6091</v>
+        <v>16.4362</v>
       </c>
       <c r="F87" t="n">
-        <v>-9.526300000000001</v>
-      </c>
-      <c r="G87" t="n">
-        <v>3.6244</v>
-      </c>
-      <c r="H87" t="n">
-        <v>-4.6764</v>
-      </c>
-      <c r="I87" t="n">
-        <v>0.9692</v>
+        <v>-15.4362</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="n">
-        <v>0.7539</v>
+        <v>0.763</v>
       </c>
       <c r="B88" t="n">
-        <v>1.0873</v>
+        <v>5.0689</v>
       </c>
       <c r="C88" t="n">
-        <v>-1.0195</v>
+        <v>-37.7777</v>
       </c>
       <c r="D88" t="n">
-        <v>0.6749000000000001</v>
+        <v>0.1416</v>
       </c>
       <c r="E88" t="n">
-        <v>10.8598</v>
+        <v>16.8659</v>
       </c>
       <c r="F88" t="n">
-        <v>-9.7599</v>
-      </c>
-      <c r="G88" t="n">
-        <v>3.7029</v>
-      </c>
-      <c r="H88" t="n">
-        <v>-4.8006</v>
-      </c>
-      <c r="I88" t="n">
-        <v>0.9979</v>
+        <v>-15.8659</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="n">
-        <v>0.7702</v>
+        <v>0.7786</v>
       </c>
       <c r="B89" t="n">
-        <v>1.114</v>
+        <v>5.2016</v>
       </c>
       <c r="C89" t="n">
-        <v>-1.0914</v>
+        <v>-39.8069</v>
       </c>
       <c r="D89" t="n">
-        <v>0.6734</v>
+        <v>0.141</v>
       </c>
       <c r="E89" t="n">
-        <v>11.1135</v>
+        <v>17.3013</v>
       </c>
       <c r="F89" t="n">
-        <v>-9.9964</v>
-      </c>
-      <c r="G89" t="n">
-        <v>3.7823</v>
-      </c>
-      <c r="H89" t="n">
-        <v>-4.9263</v>
-      </c>
-      <c r="I89" t="n">
-        <v>1.0268</v>
+        <v>-16.3013</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="n">
-        <v>0.7866</v>
+        <v>0.7944</v>
       </c>
       <c r="B90" t="n">
-        <v>1.1411</v>
+        <v>5.3361</v>
       </c>
       <c r="C90" t="n">
-        <v>-1.1664</v>
+        <v>-41.916</v>
       </c>
       <c r="D90" t="n">
-        <v>0.6719000000000001</v>
+        <v>0.1404</v>
       </c>
       <c r="E90" t="n">
-        <v>11.3704</v>
+        <v>17.7422</v>
       </c>
       <c r="F90" t="n">
-        <v>-10.2357</v>
-      </c>
-      <c r="G90" t="n">
-        <v>3.8628</v>
-      </c>
-      <c r="H90" t="n">
-        <v>-5.0536</v>
-      </c>
-      <c r="I90" t="n">
-        <v>1.0562</v>
+        <v>-16.7422</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="n">
-        <v>0.8033</v>
+        <v>0.8105</v>
       </c>
       <c r="B91" t="n">
-        <v>1.1684</v>
+        <v>5.4722</v>
       </c>
       <c r="C91" t="n">
-        <v>-1.2445</v>
+        <v>-44.1071</v>
       </c>
       <c r="D91" t="n">
-        <v>0.6704</v>
+        <v>0.1399</v>
       </c>
       <c r="E91" t="n">
-        <v>11.6303</v>
+        <v>18.1887</v>
       </c>
       <c r="F91" t="n">
-        <v>-10.478</v>
-      </c>
-      <c r="G91" t="n">
-        <v>3.9442</v>
-      </c>
-      <c r="H91" t="n">
-        <v>-5.1824</v>
-      </c>
-      <c r="I91" t="n">
-        <v>1.0859</v>
+        <v>-17.1887</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="n">
-        <v>0.8202</v>
+        <v>0.8267</v>
       </c>
       <c r="B92" t="n">
-        <v>1.1961</v>
+        <v>5.61</v>
       </c>
       <c r="C92" t="n">
-        <v>-1.3259</v>
+        <v>-46.3823</v>
       </c>
       <c r="D92" t="n">
-        <v>0.669</v>
+        <v>0.1393</v>
       </c>
       <c r="E92" t="n">
-        <v>11.8934</v>
+        <v>18.6408</v>
       </c>
       <c r="F92" t="n">
-        <v>-10.7232</v>
-      </c>
-      <c r="G92" t="n">
-        <v>4.0266</v>
-      </c>
-      <c r="H92" t="n">
-        <v>-5.3127</v>
-      </c>
-      <c r="I92" t="n">
-        <v>1.1159</v>
+        <v>-17.6408</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="n">
-        <v>0.8373</v>
+        <v>0.8431</v>
       </c>
       <c r="B93" t="n">
-        <v>1.2242</v>
+        <v>5.7496</v>
       </c>
       <c r="C93" t="n">
-        <v>-1.4106</v>
+        <v>-48.7436</v>
       </c>
       <c r="D93" t="n">
-        <v>0.6676</v>
+        <v>0.1388</v>
       </c>
       <c r="E93" t="n">
-        <v>12.1596</v>
+        <v>19.0985</v>
       </c>
       <c r="F93" t="n">
-        <v>-10.9713</v>
-      </c>
-      <c r="G93" t="n">
-        <v>4.11</v>
-      </c>
-      <c r="H93" t="n">
-        <v>-5.4446</v>
-      </c>
-      <c r="I93" t="n">
-        <v>1.1463</v>
+        <v>-18.0985</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="n">
-        <v>0.8546</v>
+        <v>0.8598</v>
       </c>
       <c r="B94" t="n">
-        <v>1.2526</v>
+        <v>5.8908</v>
       </c>
       <c r="C94" t="n">
-        <v>-1.4988</v>
+        <v>-51.1932</v>
       </c>
       <c r="D94" t="n">
-        <v>0.6663</v>
+        <v>0.1383</v>
       </c>
       <c r="E94" t="n">
-        <v>12.4289</v>
+        <v>19.5617</v>
       </c>
       <c r="F94" t="n">
-        <v>-11.2223</v>
-      </c>
-      <c r="G94" t="n">
-        <v>4.1944</v>
-      </c>
-      <c r="H94" t="n">
-        <v>-5.5781</v>
-      </c>
-      <c r="I94" t="n">
-        <v>1.1771</v>
+        <v>-18.5617</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="n">
-        <v>0.872</v>
+        <v>0.8766</v>
       </c>
       <c r="B95" t="n">
-        <v>1.2813</v>
+        <v>6.0338</v>
       </c>
       <c r="C95" t="n">
-        <v>-1.5905</v>
+        <v>-53.7333</v>
       </c>
       <c r="D95" t="n">
-        <v>0.665</v>
+        <v>0.1378</v>
       </c>
       <c r="E95" t="n">
-        <v>12.7014</v>
+        <v>20.0305</v>
       </c>
       <c r="F95" t="n">
-        <v>-11.4762</v>
-      </c>
-      <c r="G95" t="n">
-        <v>4.2797</v>
-      </c>
-      <c r="H95" t="n">
-        <v>-5.713</v>
-      </c>
-      <c r="I95" t="n">
-        <v>1.2082</v>
+        <v>-19.0305</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="n">
-        <v>0.8897</v>
+        <v>0.8935999999999999</v>
       </c>
       <c r="B96" t="n">
-        <v>1.3103</v>
+        <v>6.1784</v>
       </c>
       <c r="C96" t="n">
-        <v>-1.6857</v>
+        <v>-56.3661</v>
       </c>
       <c r="D96" t="n">
-        <v>0.6637</v>
+        <v>0.1374</v>
       </c>
       <c r="E96" t="n">
-        <v>12.9769</v>
+        <v>20.5048</v>
       </c>
       <c r="F96" t="n">
-        <v>-11.7331</v>
-      </c>
-      <c r="G96" t="n">
-        <v>4.366</v>
-      </c>
-      <c r="H96" t="n">
-        <v>-5.8496</v>
-      </c>
-      <c r="I96" t="n">
-        <v>1.2397</v>
+        <v>-19.5048</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="n">
-        <v>0.9076</v>
+        <v>0.9109</v>
       </c>
       <c r="B97" t="n">
-        <v>1.3397</v>
+        <v>6.3248</v>
       </c>
       <c r="C97" t="n">
-        <v>-1.7847</v>
+        <v>-59.0937</v>
       </c>
       <c r="D97" t="n">
-        <v>0.6625</v>
+        <v>0.1369</v>
       </c>
       <c r="E97" t="n">
-        <v>13.2556</v>
+        <v>20.9848</v>
       </c>
       <c r="F97" t="n">
-        <v>-11.9928</v>
-      </c>
-      <c r="G97" t="n">
-        <v>4.4533</v>
-      </c>
-      <c r="H97" t="n">
-        <v>-5.9876</v>
-      </c>
-      <c r="I97" t="n">
-        <v>1.2715</v>
+        <v>-19.9848</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="n">
-        <v>0.9257</v>
+        <v>0.9283</v>
       </c>
       <c r="B98" t="n">
-        <v>1.3695</v>
+        <v>6.4729</v>
       </c>
       <c r="C98" t="n">
-        <v>-1.8874</v>
+        <v>-61.9185</v>
       </c>
       <c r="D98" t="n">
-        <v>0.6613</v>
+        <v>0.1365</v>
       </c>
       <c r="E98" t="n">
-        <v>13.5374</v>
+        <v>21.4703</v>
       </c>
       <c r="F98" t="n">
-        <v>-12.2554</v>
-      </c>
-      <c r="G98" t="n">
-        <v>4.5416</v>
-      </c>
-      <c r="H98" t="n">
-        <v>-6.1272</v>
-      </c>
-      <c r="I98" t="n">
-        <v>1.3037</v>
+        <v>-20.4703</v>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="n">
-        <v>0.944</v>
+        <v>0.9459</v>
       </c>
       <c r="B99" t="n">
-        <v>1.3995</v>
+        <v>6.6226</v>
       </c>
       <c r="C99" t="n">
-        <v>-1.994</v>
+        <v>-64.8426</v>
       </c>
       <c r="D99" t="n">
-        <v>0.6602</v>
+        <v>0.136</v>
       </c>
       <c r="E99" t="n">
-        <v>13.8223</v>
+        <v>21.9613</v>
       </c>
       <c r="F99" t="n">
-        <v>-12.5209</v>
-      </c>
-      <c r="G99" t="n">
-        <v>4.6308</v>
-      </c>
-      <c r="H99" t="n">
-        <v>-6.2684</v>
-      </c>
-      <c r="I99" t="n">
-        <v>1.3362</v>
+        <v>-20.9613</v>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="n">
-        <v>0.9624</v>
+        <v>0.9637</v>
       </c>
       <c r="B100" t="n">
-        <v>1.4299</v>
+        <v>6.7741</v>
       </c>
       <c r="C100" t="n">
-        <v>-2.1046</v>
+        <v>-67.86839999999999</v>
       </c>
       <c r="D100" t="n">
-        <v>0.6591</v>
+        <v>0.1356</v>
       </c>
       <c r="E100" t="n">
-        <v>14.1103</v>
+        <v>22.458</v>
       </c>
       <c r="F100" t="n">
-        <v>-12.7894</v>
-      </c>
-      <c r="G100" t="n">
-        <v>4.721</v>
-      </c>
-      <c r="H100" t="n">
-        <v>-6.4111</v>
-      </c>
-      <c r="I100" t="n">
-        <v>1.3691</v>
+        <v>-21.458</v>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="n">
-        <v>0.9811</v>
+        <v>0.9818</v>
       </c>
       <c r="B101" t="n">
-        <v>1.4607</v>
+        <v>6.9272</v>
       </c>
       <c r="C101" t="n">
-        <v>-2.2192</v>
+        <v>-70.9982</v>
       </c>
       <c r="D101" t="n">
-        <v>0.658</v>
+        <v>0.1352</v>
       </c>
       <c r="E101" t="n">
-        <v>14.4015</v>
+        <v>22.9602</v>
       </c>
       <c r="F101" t="n">
-        <v>-13.0607</v>
-      </c>
-      <c r="G101" t="n">
-        <v>4.8122</v>
-      </c>
-      <c r="H101" t="n">
-        <v>-6.5554</v>
-      </c>
-      <c r="I101" t="n">
-        <v>1.4024</v>
+        <v>-21.9602</v>
       </c>
     </row>
     <row r="102">
@@ -29352,28 +28445,19 @@
         <v>1</v>
       </c>
       <c r="B102" t="n">
-        <v>1.4917</v>
+        <v>7.0821</v>
       </c>
       <c r="C102" t="n">
-        <v>-2.3379</v>
+        <v>-74.23439999999999</v>
       </c>
       <c r="D102" t="n">
-        <v>0.657</v>
+        <v>0.1348</v>
       </c>
       <c r="E102" t="n">
-        <v>14.6957</v>
+        <v>23.468</v>
       </c>
       <c r="F102" t="n">
-        <v>-13.335</v>
-      </c>
-      <c r="G102" t="n">
-        <v>4.9044</v>
-      </c>
-      <c r="H102" t="n">
-        <v>-6.7011</v>
-      </c>
-      <c r="I102" t="n">
-        <v>1.436</v>
+        <v>-22.468</v>
       </c>
     </row>
   </sheetData>

</xml_diff>